<commit_message>
fix: swap Turkey-Türkiye terminology mapping logic and sync
</commit_message>
<xml_diff>
--- a/step3_noise_generation/error_reports_xlsx/common_errors.xlsx
+++ b/step3_noise_generation/error_reports_xlsx/common_errors.xlsx
@@ -456,22 +456,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>buisness</t>
+          <t>succesful</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>business</t>
+          <t>successful</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Childhood friends Bill Gates and Paul Allen sought to make a buisness using their skills in computer programming.</t>
+          <t>After two uncertain years in India, where he was unable to start a succesful law practice, Gandhi moved to South Africa in 1893 to represent an Indian merchant in a lawsuit.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Childhood friends Bill Gates and Paul Allen sought to make a business using their skills in computer programming.</t>
+          <t>After two uncertain years in India, where he was unable to start a successful law practice, Gandhi moved to South Africa in 1893 to represent an Indian merchant in a lawsuit.</t>
         </is>
       </c>
     </row>
@@ -483,22 +483,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>goverment.</t>
+          <t>socio-politcal</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>government.</t>
+          <t>socio-political</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>In many systems, the prime minister selects and may dismiss other members of the cabinet, and allocates posts to members within the goverment.</t>
+          <t>Ideologically a secularist, republican and nationalist, his policies and socio-politcal theories became known as Kemalism.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>In many systems, the prime minister selects and may dismiss other members of the cabinet, and allocates posts to members within the government.</t>
+          <t>Ideologically a secularist, republican and nationalist, his policies and socio-political theories became known as Kemalism.</t>
         </is>
       </c>
     </row>
@@ -510,22 +510,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>goverment,</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>government,</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>After two years out of Parliament, he was Chancellor of the Exchequer in Stanley Baldwin's Conservative goverment, returning sterling in 1925 to the gold standard, depressing the UK economy.</t>
+          <t>Leaders of politcal parties are generally expected to run as a presidential candidate for their party.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>After two years out of Parliament, he was Chancellor of the Exchequer in Stanley Baldwin's Conservative government, returning sterling in 1925 to the gold standard, depressing the UK economy.</t>
+          <t>Leaders of political parties are generally expected to run as a presidential candidate for their party.</t>
         </is>
       </c>
     </row>
@@ -537,22 +537,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>goverment,</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>government,</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>As chief officer of municipal goverment, the sovereign had duties and responsibilities deriving from the charter which established the local town borough or council.</t>
+          <t>Since 2015, Trump's leadership style and politcal agenda—often referred to as Trumpism—have reshaped the Republican Party's identity.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>As chief officer of municipal government, the sovereign had duties and responsibilities deriving from the charter which established the local town borough or council.</t>
+          <t>Since 2015, Trump's leadership style and political agenda—often referred to as Trumpism—have reshaped the Republican Party's identity.</t>
         </is>
       </c>
     </row>
@@ -574,12 +574,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Mohandas Karamchand Gandhi (2 October 1869 – 30 January 1948) was an Indian lawyer, anti-colonial nationalist, and politcal thinker who employed nonviolent resistance to lead the successful campaign for India's independence from British rule.</t>
+          <t>Judges constitute a critical force for judicial interpretation and constitutional review while avoiding politcal bias.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Mohandas Karamchand Gandhi (2 October 1869 – 30 January 1948) was an Indian lawyer, anti-colonial nationalist, and political thinker who employed nonviolent resistance to lead the successful campaign for India's independence from British rule.</t>
+          <t>Judges constitute a critical force for judicial interpretation and constitutional review while avoiding political bias.</t>
         </is>
       </c>
     </row>
@@ -591,22 +591,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>proffesional</t>
+          <t>self-goverment</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>professional</t>
+          <t>self-government</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>A proffesional practitioner or researcher involved in the discipline is called a psychologist.</t>
+          <t>Parliament responded by enacting a series of punitive laws, which effectively ended self-goverment in Massachusetts, but also intensified support for the revolutionary cause among Americans.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>A professional practitioner or researcher involved in the discipline is called a psychologist.</t>
+          <t>Parliament responded by enacting a series of punitive laws, which effectively ended self-government in Massachusetts, but also intensified support for the revolutionary cause among Americans.</t>
         </is>
       </c>
     </row>
@@ -628,12 +628,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>During the Constitutional Convention, delegates opposed to having a strong central goverment argued that national laws could be enforced by state courts.</t>
+          <t>The president of South Africa is the head of state and head of goverment of the Republic of South Africa.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>During the Constitutional Convention, delegates opposed to having a strong central government argued that national laws could be enforced by state courts.</t>
+          <t>The president of South Africa is the head of state and head of government of the Republic of South Africa.</t>
         </is>
       </c>
     </row>
@@ -645,22 +645,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>politcal</t>
+          <t>buisness</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>political</t>
+          <t>business</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>He led an invasion of Egypt and Syria in 1798, which served as a springboard to politcal power.</t>
+          <t>In 2023, Trump was found liable in civil cases for sexual abuse and defamation and for buisness fraud.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>He led an invasion of Egypt and Syria in 1798, which served as a springboard to political power.</t>
+          <t>In 2023, Trump was found liable in civil cases for sexual abuse and defamation and for business fraud.</t>
         </is>
       </c>
     </row>
@@ -672,22 +672,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>begining</t>
+          <t>goverment.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>beginning</t>
+          <t>government.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Day was established as a holiday in cities and states throughout the United States begining in 1971; the federal holiday was first observed in 1986.</t>
+          <t>Executive power is exercised by the Council of Ministers, which is appointed and headed by the President, who serves as country's head of state and head of goverment.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Day was established as a holiday in cities and states throughout the United States beginning in 1971; the federal holiday was first observed in 1986.</t>
+          <t>Executive power is exercised by the Council of Ministers, which is appointed and headed by the President, who serves as country's head of state and head of government.</t>
         </is>
       </c>
     </row>
@@ -699,22 +699,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>begining</t>
+          <t>enviroment</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Beginning</t>
+          <t>environment</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>begining in 1299, the Ottomans united the principalities and expanded.</t>
+          <t>Sanctions on the enviroment – since the declaration of the United Nations Conference on the Human Environment, international environmental protection efforts have been increased gradually.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Beginning in 1299, the Ottomans united the principalities and expanded.</t>
+          <t>Sanctions on the environment – since the declaration of the United Nations Conference on the Human Environment, international environmental protection efforts have been increased gradually.</t>
         </is>
       </c>
     </row>
@@ -736,12 +736,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>A legislature (UK:, US: ) is a deliberative assembly that holds the legal authority to make law and exercise politcal oversight within a political entity such as a state, nation, or city.</t>
+          <t>Thematic categorizations include politcal history, military history, social history, and economic history.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>A legislature (UK:, US: ) is a deliberative assembly that holds the legal authority to make law and exercise political oversight within a political entity such as a state, nation, or city.</t>
+          <t>Thematic categorizations include political history, military history, social history, and economic history.</t>
         </is>
       </c>
     </row>
@@ -758,17 +758,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>political</t>
+          <t>Political</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>As a member of the Committee of Union and Progress and the Young Turks, he played an important part in politcal events of the late Ottoman Empire, such as the Young Turk Revolution and the 31 March Incident.</t>
+          <t>politcal parties in different countries will often adopt similar colours and symbols to identify themselves with a particular ideology.</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>As a member of the Committee of Union and Progress and the Young Turks, he played an important part in political events of the late Ottoman Empire, such as the Young Turk Revolution and the 31 March Incident.</t>
+          <t>Political parties in different countries will often adopt similar colours and symbols to identify themselves with a particular ideology.</t>
         </is>
       </c>
     </row>
@@ -780,22 +780,22 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>begining</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>beginning</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>They developed the first known codified legal and administrative systems, complete with courts, jails, and goverment records.</t>
+          <t>The Sultan, begining in 1517, was also a caliph, the leader of all the Sunni Muslims in the world.</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>They developed the first known codified legal and administrative systems, complete with courts, jails, and government records.</t>
+          <t>The Sultan, beginning in 1517, was also a caliph, the leader of all the Sunni Muslims in the world.</t>
         </is>
       </c>
     </row>
@@ -807,22 +807,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>politcal,</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>political,</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>They encompass a broad range of civil, politcal, economic, social, and cultural rights, such as the right to life, freedom of speech, protection against enslavement, and right to education.</t>
+          <t>It developed in new directions during the European Enlightenment with such philosophers as John Locke, Francis Hutcheson, and Jean-Jacques Burlamaqui, and featured prominently in the politcal discourse of the American Revolution and the French Revolution.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>They encompass a broad range of civil, political, economic, social, and cultural rights, such as the right to life, freedom of speech, protection against enslavement, and right to education.</t>
+          <t>It developed in new directions during the European Enlightenment with such philosophers as John Locke, Francis Hutcheson, and Jean-Jacques Burlamaqui, and featured prominently in the political discourse of the American Revolution and the French Revolution.</t>
         </is>
       </c>
     </row>
@@ -834,22 +834,22 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>politcal</t>
+          <t>independant</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>political</t>
+          <t>Independent</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Conservatism has been called a "philosophy of human imperfection" by politcal scientist Noël O'Sullivan, reflecting among its adherents a negative view of human nature and pessimism of the potential to improve it through 'utopian' schemes.</t>
+          <t>independant candidates may run, and to be elected, they must only win enough to get one seat.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Conservatism has been called a "philosophy of human imperfection" by political scientist Noël O'Sullivan, reflecting among its adherents a negative view of human nature and pessimism of the potential to improve it through 'utopian' schemes.</t>
+          <t>Independent candidates may run, and to be elected, they must only win enough to get one seat.</t>
         </is>
       </c>
     </row>
@@ -861,22 +861,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>politcal</t>
+          <t>proffesional</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>political</t>
+          <t>professional</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Depending on the academic institution, international relations or international affairs is either a subdiscipline of politcal science or a broader multidisciplinary field encompassing global politics, law, economics, or world history.</t>
+          <t>The Faculty of Arts and Sciences offers study in a wide range of undergraduate and graduate academic disciplines, and other faculties offer graduate degrees, including proffesional degrees.</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Depending on the academic institution, international relations or international affairs is either a subdiscipline of political science or a broader multidisciplinary field encompassing global politics, law, economics, or world history.</t>
+          <t>The Faculty of Arts and Sciences offers study in a wide range of undergraduate and graduate academic disciplines, and other faculties offer graduate degrees, including professional degrees.</t>
         </is>
       </c>
     </row>
@@ -898,12 +898,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>From 1961 until 2017, Turkish presidents were required to sever all relations, if any, with their politcal party.</t>
+          <t>Presenting himself as a politcal outsider, Trump won the 2016 presidential election against Democratic Party nominee Hillary Clinton.</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>From 1961 until 2017, Turkish presidents were required to sever all relations, if any, with their political party.</t>
+          <t>Presenting himself as a political outsider, Trump won the 2016 presidential election against Democratic Party nominee Hillary Clinton.</t>
         </is>
       </c>
     </row>
@@ -915,22 +915,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>goverment,</t>
+          <t>immediatly.</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>government,</t>
+          <t>immediately.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>As well as being head of goverment, being prime minister may require holding other roles or posts—the prime minister of the United Kingdom, for example, is also First Lord of the Treasury and Minister for the Civil Service.</t>
+          <t>If the National Assembly votes against a presidential decision, it will be declared void immediatly.</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>As well as being head of government, being prime minister may require holding other roles or posts—the prime minister of the United Kingdom, for example, is also First Lord of the Treasury and Minister for the Civil Service.</t>
+          <t>If the National Assembly votes against a presidential decision, it will be declared void immediately.</t>
         </is>
       </c>
     </row>
@@ -942,22 +942,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>independant</t>
+          <t>self-goverment</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>independent</t>
+          <t>self-government</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>The period between roughly 1500 to 1789 saw the rise of independant sovereign states, multilateralism, and the institutionalization of diplomacy and the military.</t>
+          <t>Federalists fought for complete self-goverment and full provincial autonomy, as opposed to the centralized government that the Unitarians and Centralists favored.</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>The period between roughly 1500 to 1789 saw the rise of independent sovereign states, multilateralism, and the institutionalization of diplomacy and the military.</t>
+          <t>Federalists fought for complete self-government and full provincial autonomy, as opposed to the centralized government that the Unitarians and Centralists favored.</t>
         </is>
       </c>
     </row>
@@ -969,22 +969,22 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>self-goverment</t>
+          <t>enviroment</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>self-government</t>
+          <t>environment</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Federalists fought for complete self-goverment and full provincial autonomy, as opposed to the centralized government that the Unitarians and Centralists favored.</t>
+          <t>Small uncrewed spacecraft can also provide platforms for experiments, especially those involving zero gravity and exposure to space, but space stations offer a long-term enviroment where studies can be performed potentially for decades, combined with ready access by human researchers.</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Federalists fought for complete self-government and full provincial autonomy, as opposed to the centralized government that the Unitarians and Centralists favored.</t>
+          <t>Small uncrewed spacecraft can also provide platforms for experiments, especially those involving zero gravity and exposure to space, but space stations offer a long-term environment where studies can be performed potentially for decades, combined with ready access by human researchers.</t>
         </is>
       </c>
     </row>
@@ -1006,12 +1006,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>In parallel, many former socialist politicians and politcal parties embraced "Third Way" politics, remaining committed to equality and welfare while abandoning public ownership and class-based politics.</t>
+          <t>Institutions are also a central concern for law, the formal mechanism for politcal rule-making and enforcement.</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>In parallel, many former socialist politicians and political parties embraced "Third Way" politics, remaining committed to equality and welfare while abandoning public ownership and class-based politics.</t>
+          <t>Institutions are also a central concern for law, the formal mechanism for political rule-making and enforcement.</t>
         </is>
       </c>
     </row>
@@ -1023,22 +1023,22 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>goverment,</t>
+          <t>immediatly,</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>government,</t>
+          <t>immediately,</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>A sitting president (or governor or mayor) who wishes to run for a different office, regardless of the intended jurisdiction or branch of goverment, must resign from office at least six months before election day.</t>
+          <t>A provisional measure comes into effect immediatly, before Congress votes on it, and remains in force for up to 60 days unless Congress votes to rescind it.</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>A sitting president (or governor or mayor) who wishes to run for a different office, regardless of the intended jurisdiction or branch of government, must resign from office at least six months before election day.</t>
+          <t>A provisional measure comes into effect immediately, before Congress votes on it, and remains in force for up to 60 days unless Congress votes to rescind it.</t>
         </is>
       </c>
     </row>
@@ -1050,22 +1050,22 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>goverment,</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>government,</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Out of goverment during his so-called "wilderness years" in the 1930s, Churchill took the lead in calling for rearmament to counter the threat of militarism in Nazi Germany.</t>
+          <t>If the leader of the opposition is unable or unwilling to form a goverment, the governor general can consult whomever they wish.</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Out of government during his so-called "wilderness years" in the 1930s, Churchill took the lead in calling for rearmament to counter the threat of militarism in Nazi Germany.</t>
+          <t>If the leader of the opposition is unable or unwilling to form a government, the governor general can consult whomever they wish.</t>
         </is>
       </c>
     </row>
@@ -1077,22 +1077,22 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>goverment,</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Government</t>
+          <t>government,</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>A nationalist goverment of the Grand National Assembly (GNA) led by Mustafa Kemal was established in Ankara when it became clear the Ottoman government was backing the Allied powers.</t>
+          <t>From the 1990s, many Communist parties adopted democratic principles and came to share power with others in goverment, such as the CPN UML and the Nepal Communist Party, which support People's Multiparty Democracy in Nepal.</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>A nationalist Government of the Grand National Assembly (GNA) led by Mustafa Kemal was established in Ankara when it became clear the Ottoman government was backing the Allied powers.</t>
+          <t>From the 1990s, many Communist parties adopted democratic principles and came to share power with others in government, such as the CPN UML and the Nepal Communist Party, which support People's Multiparty Democracy in Nepal.</t>
         </is>
       </c>
     </row>
@@ -1104,22 +1104,22 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>immediatly</t>
+          <t>enviroment</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>immediately</t>
+          <t>environment</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Due to the previous president's impeachment and expulsion from office, Lee was sworn in immediatly the next day.</t>
+          <t>This enviroment encompasses the interaction of all living species, climate, weather and natural resources that affect human survival and economic activity.</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Due to the previous president's impeachment and expulsion from office, Lee was sworn in immediately the next day.</t>
+          <t>This environment encompasses the interaction of all living species, climate, weather and natural resources that affect human survival and economic activity.</t>
         </is>
       </c>
     </row>
@@ -1131,22 +1131,22 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>begining</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>beginning</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>The separation of powers principle functionally differentiates several types of state power (usually legislation, adjudication, and execution) and requires these operations of goverment to be conceptually and institutionally distinct and clearly articulated, thereby maintaining the integrity of each branch.</t>
+          <t>While initially committing to democratic governance, Vargas assumed dictatorial powers following a self-coup in 1937, marking the begining of the Estado Novo, in which he oversaw Brazil's involvement in World War II.</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>The separation of powers principle functionally differentiates several types of state power (usually legislation, adjudication, and execution) and requires these operations of government to be conceptually and institutionally distinct and clearly articulated, thereby maintaining the integrity of each branch.</t>
+          <t>While initially committing to democratic governance, Vargas assumed dictatorial powers following a self-coup in 1937, marking the beginning of the Estado Novo, in which he oversaw Brazil's involvement in World War II.</t>
         </is>
       </c>
     </row>
@@ -1158,22 +1158,22 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>succesful</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>successful</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>On 2 March 2025, Firefly Aerospace's Blue Ghost lunar lander made the first fully succesful commercial Moon landing after softly landing upright near Mons Latreille in Mare Crisium.</t>
+          <t>Mohandas Karamchand Gandhi (2 October 1869 – 30 January 1948) was an Indian lawyer, anti-colonial nationalist, and politcal thinker who employed nonviolent resistance to lead the successful campaign for India's independence from British rule.</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>On 2 March 2025, Firefly Aerospace's Blue Ghost lunar lander made the first fully successful commercial Moon landing after softly landing upright near Mons Latreille in Mare Crisium.</t>
+          <t>Mohandas Karamchand Gandhi (2 October 1869 – 30 January 1948) was an Indian lawyer, anti-colonial nationalist, and political thinker who employed nonviolent resistance to lead the successful campaign for India's independence from British rule.</t>
         </is>
       </c>
     </row>
@@ -1185,22 +1185,22 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>enviroment</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>environment</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>It is a field of research in computer science that develops and studies methods and software that enable machines to perceive their enviroment and use learning and intelligence to take actions that maximize their chances of achieving defined goals.</t>
+          <t>The main types of modern politcal systems recognized are democracies, totalitarian regimes, and, sitting between these two, authoritarian regimes with a variety of hybrid regimes.</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>It is a field of research in computer science that develops and studies methods and software that enable machines to perceive their environment and use learning and intelligence to take actions that maximize their chances of achieving defined goals.</t>
+          <t>The main types of modern political systems recognized are democracies, totalitarian regimes, and, sitting between these two, authoritarian regimes with a variety of hybrid regimes.</t>
         </is>
       </c>
     </row>
@@ -1212,22 +1212,22 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>independant</t>
+          <t>seperate</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>independent</t>
+          <t>separate</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>The absence of powerful states in Greece after the collapse of Mycenaean power, and the geography of Greece, where many settlements were separated from their neighbours by mountainous terrain, encouraged the development of small independant city-states.</t>
+          <t>However, they are considered seperate academic disciplines in the modern sense of the term.</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>The absence of powerful states in Greece after the collapse of Mycenaean power, and the geography of Greece, where many settlements were separated from their neighbours by mountainous terrain, encouraged the development of small independent city-states.</t>
+          <t>However, they are considered separate academic disciplines in the modern sense of the term.</t>
         </is>
       </c>
     </row>
@@ -1249,12 +1249,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>In the 2009 federal election, the CDU obtained the largest share of the vote, and Merkel subsequently formed a coalition goverment with the Free Democratic Party (FDP), an alliance more favourable to the CDU than the grand coalition.</t>
+          <t>Generally, a parliament has three functions: representing the electorate, making laws, and overseeing the executive goverment via hearings and inquiries.</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>In the 2009 federal election, the CDU obtained the largest share of the vote, and Merkel subsequently formed a coalition government with the Free Democratic Party (FDP), an alliance more favourable to the CDU than the grand coalition.</t>
+          <t>Generally, a parliament has three functions: representing the electorate, making laws, and overseeing the executive government via hearings and inquiries.</t>
         </is>
       </c>
     </row>
@@ -1266,22 +1266,22 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>After the National Party's white-only goverment established apartheid, a system of racial segregation that privileged whites, Mandela and the ANC committed themselves to its overthrow.</t>
+          <t>He began to live in a self-sufficient residential community, to eat simple food, and undertake long fasts as a means of both introspection and politcal protest.</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>After the National Party's white-only government established apartheid, a system of racial segregation that privileged whites, Mandela and the ANC committed themselves to its overthrow.</t>
+          <t>He began to live in a self-sufficient residential community, to eat simple food, and undertake long fasts as a means of both introspection and political protest.</t>
         </is>
       </c>
     </row>
@@ -1293,22 +1293,22 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Government</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>goverment restrictions on freedom of the press may include classified information, state secrets, punishment for libel, punishment for violation of copyright, privacy, or judicial orders.</t>
+          <t>A faith in custom, convention, and prescription, and a recognition that innovation must be tied to existing traditions and customs, which entails a respect for the politcal value of prudence.</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Government restrictions on freedom of the press may include classified information, state secrets, punishment for libel, punishment for violation of copyright, privacy, or judicial orders.</t>
+          <t>A faith in custom, convention, and prescription, and a recognition that innovation must be tied to existing traditions and customs, which entails a respect for the political value of prudence.</t>
         </is>
       </c>
     </row>
@@ -1320,22 +1320,22 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>politcal</t>
+          <t>goverment</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>political</t>
+          <t>government</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>As a moderate Republican, Lincoln had to navigate conflicting politcal opinions from contentious factions during the war effort.</t>
+          <t>Chapter III of Title III of the Constitution deals with the executive branch of goverment and sets forth the powers of the president, as well as the qualifications for the office.</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>As a moderate Republican, Lincoln had to navigate conflicting political opinions from contentious factions during the war effort.</t>
+          <t>Chapter III of Title III of the Constitution deals with the executive branch of government and sets forth the powers of the president, as well as the qualifications for the office.</t>
         </is>
       </c>
     </row>
@@ -1347,22 +1347,22 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>politcal,</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>political,</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>It describes the economic, politcal, and social theories and movements associated with the implementation of such systems.</t>
+          <t>Turkish women received equal civil and politcal rights during his presidency.</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>It describes the economic, political, and social theories and movements associated with the implementation of such systems.</t>
+          <t>Turkish women received equal civil and political rights during his presidency.</t>
         </is>
       </c>
     </row>
@@ -1374,22 +1374,22 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>politcal,</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>political,</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Panels of experts assess the press freedom score and draft each country summary according to a weighted scoring system that analyzes the politcal, economic, legal and safety situation for journalists based on a 100-point scale.</t>
+          <t>By the turn of the 19th century the Ottoman ruling elite recognized the need to restructure the legislative, military and judiciary systems to cope with their new politcal rivals in Europe.</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Panels of experts assess the press freedom score and draft each country summary according to a weighted scoring system that analyzes the political, economic, legal and safety situation for journalists based on a 100-point scale.</t>
+          <t>By the turn of the 19th century the Ottoman ruling elite recognized the need to restructure the legislative, military and judiciary systems to cope with their new political rivals in Europe.</t>
         </is>
       </c>
     </row>
@@ -1401,22 +1401,22 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>begining</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>beginning</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Proponents of a "long Renaissance" may put its begining in the 14th century and its end in the 17th century.</t>
+          <t>There are many different ways in which politcal parties can be structured and interact with the electorate.</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Proponents of a "long Renaissance" may put its beginning in the 14th century and its end in the 17th century.</t>
+          <t>There are many different ways in which political parties can be structured and interact with the electorate.</t>
         </is>
       </c>
     </row>
@@ -1428,22 +1428,22 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>politcal</t>
+          <t>independant</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Political</t>
+          <t>independent</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>politcal scientists have sometimes defined institutions in more formal ways where third parties must reliably and predictably enforce the rules governing the transactions of first and second parties.</t>
+          <t>The absence of powerful states in Greece after the collapse of Mycenaean power, and the geography of Greece, where many settlements were separated from their neighbours by mountainous terrain, encouraged the development of small independant city-states.</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Political scientists have sometimes defined institutions in more formal ways where third parties must reliably and predictably enforce the rules governing the transactions of first and second parties.</t>
+          <t>The absence of powerful states in Greece after the collapse of Mycenaean power, and the geography of Greece, where many settlements were separated from their neighbours by mountainous terrain, encouraged the development of small independent city-states.</t>
         </is>
       </c>
     </row>
@@ -1455,22 +1455,22 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>enviroment,</t>
+          <t>goverment</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>environment,</t>
+          <t>government</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>More precisely, we can consider the different aspects or components of an enviroment, and see that their degree of naturalness is not uniform.</t>
+          <t>Article II of the Constitution establishes the executive branch of the federal goverment and vests executive power in the president.</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>More precisely, we can consider the different aspects or components of an environment, and see that their degree of naturalness is not uniform.</t>
+          <t>Article II of the Constitution establishes the executive branch of the federal government and vests executive power in the president.</t>
         </is>
       </c>
     </row>
@@ -1482,22 +1482,22 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Another example is the Thirty-fourth goverment of Israel (2015–2019), when Benjamin Netanyahu at one point served as the prime minister and minister of Communications, Foreign Affairs, Regional Cooperation, Economy, Defense and Interior.</t>
+          <t>The position of prime minister was not created but evolved slowly and organically over three hundred years due to numerous Acts of Parliament, politcal developments, and accidents of history.</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Another example is the Thirty-fourth government of Israel (2015–2019), when Benjamin Netanyahu at one point served as the prime minister and minister of Communications, Foreign Affairs, Regional Cooperation, Economy, Defense and Interior.</t>
+          <t>The position of prime minister was not created but evolved slowly and organically over three hundred years due to numerous Acts of Parliament, political developments, and accidents of history.</t>
         </is>
       </c>
     </row>
@@ -1509,22 +1509,22 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>proffesional</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>professional</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>The position of a head of goverment separate from the head of state, or as the most important government administrator or minister after the monarch in rank developed in multiple countries separate from each other.</t>
+          <t>Following the American Civil War, under Harvard president Charles William Eliot's long tenure from 1869 to 1909, Harvard developed multiple proffesional schools, which transformed it into a modern research university.</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>The position of a head of government separate from the head of state, or as the most important government administrator or minister after the monarch in rank developed in multiple countries separate from each other.</t>
+          <t>Following the American Civil War, under Harvard president Charles William Eliot's long tenure from 1869 to 1909, Harvard developed multiple professional schools, which transformed it into a modern research university.</t>
         </is>
       </c>
     </row>
@@ -1536,22 +1536,22 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>neccessary".</t>
+          <t>begining</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>necessary".</t>
+          <t>beginning</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>The measures are limited to the "minimum neccessary".</t>
+          <t>Cultural and technological developments transformed European society, concluding the Late Middle Ages and begining the early modern period.</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>The measures are limited to the "minimum necessary".</t>
+          <t>Cultural and technological developments transformed European society, concluding the Late Middle Ages and beginning the early modern period.</t>
         </is>
       </c>
     </row>
@@ -1563,22 +1563,22 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>buisness,</t>
+          <t>goverment</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>business,</t>
+          <t>Government</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Philosophy is related to many other fields, such as the natural and social sciences, mathematics, buisness, law, and journalism.</t>
+          <t>A new National Constitution was proposed only in 1826, during the Presidency of Unitarian Bernardino Rivadavia, but it was again rejected by the Provinces, leading to the dissolution of the National goverment the following year.</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Philosophy is related to many other fields, such as the natural and social sciences, mathematics, business, law, and journalism.</t>
+          <t>A new National Constitution was proposed only in 1826, during the Presidency of Unitarian Bernardino Rivadavia, but it was again rejected by the Provinces, leading to the dissolution of the National Government the following year.</t>
         </is>
       </c>
     </row>
@@ -1600,12 +1600,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>The first Austrian sovereign head of goverment was the State Chancellor of the Austrian Empire, a position only held by Klemens von Metternich.</t>
+          <t>He implemented a strong, well-financed national goverment while remaining impartial in the fierce rivalry that emerged within his cabinet between Thomas Jefferson and Alexander Hamilton.</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>The first Austrian sovereign head of government was the State Chancellor of the Austrian Empire, a position only held by Klemens von Metternich.</t>
+          <t>He implemented a strong, well-financed national government while remaining impartial in the fierce rivalry that emerged within his cabinet between Thomas Jefferson and Alexander Hamilton.</t>
         </is>
       </c>
     </row>
@@ -1617,22 +1617,22 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>politcal</t>
+          <t>goverment</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>political</t>
+          <t>government</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>In The Spirit of Law (1748), Montesquieu described the various forms of distribution of politcal power among a legislature, an executive, and a judiciary.</t>
+          <t>While all types of organizations have governance, the term goverment is often used more specifically to refer to the approximately 200 independent national governments and subsidiary organizations.</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>In The Spirit of Law (1748), Montesquieu described the various forms of distribution of political power among a legislature, an executive, and a judiciary.</t>
+          <t>While all types of organizations have governance, the term government is often used more specifically to refer to the approximately 200 independent national governments and subsidiary organizations.</t>
         </is>
       </c>
     </row>
@@ -1644,22 +1644,22 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>The word goverment derives from the Greek verb κυβερνάω meaning to steer with a gubernaculum (rudder), the metaphorical sense being attested in the literature of classical antiquity, including Plato's Ship of State.</t>
+          <t>In many countries, the notion of a politcal party is defined in law, and governments may specify requirements for an organization to legally qualify as a political party.</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>The word government derives from the Greek verb κυβερνάω meaning to steer with a gubernaculum (rudder), the metaphorical sense being attested in the literature of classical antiquity, including Plato's Ship of State.</t>
+          <t>In many countries, the notion of a political party is defined in law, and governments may specify requirements for an organization to legally qualify as a political party.</t>
         </is>
       </c>
     </row>
@@ -1681,12 +1681,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Contemporary philosophy of law addresses problems internal to law and legal systems and problems of law as a social institution that relates to the larger politcal and social context in which it exists.</t>
+          <t>International relations is generally classified as a major multidiscipline of politcal science, along with comparative politics, political methodology, political theory, and public administration.</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Contemporary philosophy of law addresses problems internal to law and legal systems and problems of law as a social institution that relates to the larger political and social context in which it exists.</t>
+          <t>International relations is generally classified as a major multidiscipline of political science, along with comparative politics, political methodology, political theory, and public administration.</t>
         </is>
       </c>
     </row>
@@ -1698,22 +1698,22 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>independant</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>independent</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Ancient India and China represent distinct traditions of law, and had historically independant schools of legal theory and practice.</t>
+          <t>The members of a politcal party contest elections under a shared label.</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Ancient India and China represent distinct traditions of law, and had historically independent schools of legal theory and practice.</t>
+          <t>The members of a political party contest elections under a shared label.</t>
         </is>
       </c>
     </row>
@@ -1725,22 +1725,22 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>succesful</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>successful</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>In 1905, he submitted a succesful PhD dissertation to the University of Zurich.</t>
+          <t>During the preceding Middle Ages, the European organization of politcal authority was based on a vaguely hierarchical religious order.</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>In 1905, he submitted a successful PhD dissertation to the University of Zurich.</t>
+          <t>During the preceding Middle Ages, the European organization of political authority was based on a vaguely hierarchical religious order.</t>
         </is>
       </c>
     </row>
@@ -1752,22 +1752,22 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>politcal</t>
+          <t>buisness</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>political</t>
+          <t>business</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Parties are important in the politics of autocracies as well as democracies, though usually democracies have more politcal parties than autocracies.</t>
+          <t>He launched side ventures, many licensing the Trump name, and filed for six buisness bankruptcies in the 1990s and 2000s.</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Parties are important in the politics of autocracies as well as democracies, though usually democracies have more political parties than autocracies.</t>
+          <t>He launched side ventures, many licensing the Trump name, and filed for six business bankruptcies in the 1990s and 2000s.</t>
         </is>
       </c>
     </row>
@@ -1779,22 +1779,22 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Government</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>goverment is a means by which organizational policies are enforced, as well as a mechanism for determining policy.</t>
+          <t>A given economy is a set of processes that involves its culture, values, education, technological evolution, history, social organization, politcal structure, legal systems, and natural resources as main factors.</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Government is a means by which organizational policies are enforced, as well as a mechanism for determining policy.</t>
+          <t>A given economy is a set of processes that involves its culture, values, education, technological evolution, history, social organization, political structure, legal systems, and natural resources as main factors.</t>
         </is>
       </c>
     </row>
@@ -1806,22 +1806,22 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>"seperate</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>"separate</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>The presidency is a part of the system of people's congress based on the principle of unified power in which the National People's Congress (NPC) functions as the only branch of goverment and as the supreme state organ of power.</t>
+          <t>Ferguson, which established the doctrine of "seperate but equal".</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>The presidency is a part of the system of people's congress based on the principle of unified power in which the National People's Congress (NPC) functions as the only branch of government and as the supreme state organ of power.</t>
+          <t>Ferguson, which established the doctrine of "separate but equal".</t>
         </is>
       </c>
     </row>
@@ -1833,22 +1833,22 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>The powers, functions and duties of prior presidential offices, in addition to their relation with the prime minister and goverment of France, have over time differed with the various constitutional documents since the Second Republic.</t>
+          <t>A republic, based on the Latin phrase res publica ('public thing' or 'people's thing'), is a state in which politcal power rests with the public (people), typically through their representatives—in contrast to a monarchy.</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>The powers, functions and duties of prior presidential offices, in addition to their relation with the prime minister and government of France, have over time differed with the various constitutional documents since the Second Republic.</t>
+          <t>A republic, based on the Latin phrase res publica ('public thing' or 'people's thing'), is a state in which political power rests with the public (people), typically through their representatives—in contrast to a monarchy.</t>
         </is>
       </c>
     </row>
@@ -1860,22 +1860,22 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Generally, a parliament has three functions: representing the electorate, making laws, and overseeing the executive goverment via hearings and inquiries.</t>
+          <t>As a subdiscipline of politcal science, the focus of IR studies lies on the political, diplomatic, and security connections among states, as well as the study of modern international relations within the context of world history.</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Generally, a parliament has three functions: representing the electorate, making laws, and overseeing the executive government via hearings and inquiries.</t>
+          <t>As a subdiscipline of political science, the focus of IR studies lies on the political, diplomatic, and security connections among states, as well as the study of modern international relations within the context of world history.</t>
         </is>
       </c>
     </row>
@@ -1887,22 +1887,22 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>politcal</t>
+          <t>goverment</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Political</t>
+          <t>government</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>politcal parties have become a major part of the politics of almost every country, as modern party organizations developed and spread around the world over the last few centuries.</t>
+          <t>The prime minister of the United Kingdom is the head of goverment of the United Kingdom.</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Political parties have become a major part of the politics of almost every country, as modern party organizations developed and spread around the world over the last few centuries.</t>
+          <t>The prime minister of the United Kingdom is the head of government of the United Kingdom.</t>
         </is>
       </c>
     </row>
@@ -1914,22 +1914,22 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>succesful</t>
+          <t>goverment</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>successful</t>
+          <t>government</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Drafted into military service in 1958, he relaunched his recording career two years later with some of his most commercially succesful work.</t>
+          <t>Polybius explained the system of checks and balances in detail, crediting Lycurgus of Sparta with the first goverment of this kind.</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Drafted into military service in 1958, he relaunched his recording career two years later with some of his most commercially successful work.</t>
+          <t>Polybius explained the system of checks and balances in detail, crediting Lycurgus of Sparta with the first government of this kind.</t>
         </is>
       </c>
     </row>
@@ -1941,22 +1941,22 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>recieve,</t>
+          <t>buisness</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>receive,</t>
+          <t>business</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>However, in legal contexts, freedom of expression more broadly encompasses the right to seek, recieve, and impart information or ideas, regardless of the medium used.</t>
+          <t>McDonald's Corporation, doing buisness as McDonald's, is an American multinational fast food restaurant chain.</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>However, in legal contexts, freedom of expression more broadly encompasses the right to seek, receive, and impart information or ideas, regardless of the medium used.</t>
+          <t>McDonald's Corporation, doing business as McDonald's, is an American multinational fast food restaurant chain.</t>
         </is>
       </c>
     </row>
@@ -1978,12 +1978,12 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Under the interim constitution (valid from 1994 to 1996), there was a goverment of National Unity, in which a member of Parliament (MP) from the largest opposition party was entitled to a position as deputy president.</t>
+          <t>An earlier forerunner to Montesquieu's tripartite system was articulated by John Locke in his work Two Treatises of goverment (1690).</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Under the interim constitution (valid from 1994 to 1996), there was a Government of National Unity, in which a member of Parliament (MP) from the largest opposition party was entitled to a position as deputy president.</t>
+          <t>An earlier forerunner to Montesquieu's tripartite system was articulated by John Locke in his work Two Treatises of Government (1690).</t>
         </is>
       </c>
     </row>
@@ -2005,12 +2005,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Institutions are a principal object of study in social sciences such as politcal science, anthropology, economics, and sociology (the latter described by Émile Durkheim as the "science of institutions, their genesis and their functioning").</t>
+          <t>While international trade has existed throughout history (for example Uttarapatha, Silk Road, Amber Road, salt roads), its economic, social, and politcal importance has been on the rise in recent centuries.</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Institutions are a principal object of study in social sciences such as political science, anthropology, economics, and sociology (the latter described by Émile Durkheim as the "science of institutions, their genesis and their functioning").</t>
+          <t>While international trade has existed throughout history (for example Uttarapatha, Silk Road, Amber Road, salt roads), its economic, social, and political importance has been on the rise in recent centuries.</t>
         </is>
       </c>
     </row>
@@ -2022,22 +2022,22 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>goverment,</t>
+          <t>goverment</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>government,</t>
+          <t>government</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>It was used by Roman writers to refer to the state and goverment, even during the period of the Roman Empire.</t>
+          <t>The president directs the executive branch of the goverment and is the commander-in-chief of the Republic of Korea Armed Forces.</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>It was used by Roman writers to refer to the state and government, even during the period of the Roman Empire.</t>
+          <t>The president directs the executive branch of the government and is the commander-in-chief of the Republic of Korea Armed Forces.</t>
         </is>
       </c>
     </row>
@@ -2049,22 +2049,22 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>begining</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>beginning</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>The president directs the executive branch of the goverment and is the commander-in-chief of the Republic of Korea Armed Forces.</t>
+          <t>Day was established as a holiday in cities and states throughout the United States begining in 1971; the federal holiday was first observed in 1986.</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>The president directs the executive branch of the government and is the commander-in-chief of the Republic of Korea Armed Forces.</t>
+          <t>Day was established as a holiday in cities and states throughout the United States beginning in 1971; the federal holiday was first observed in 1986.</t>
         </is>
       </c>
     </row>
@@ -2076,22 +2076,22 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>politcal</t>
+          <t>goverment,</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>political</t>
+          <t>government,</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>This is related to other features that sometimes distinguish parties from other politcal organizations, including a larger membership, greater stability over time, and a deeper connection to the electorate.</t>
+          <t>It was used by Roman writers to refer to the state and goverment, even during the period of the Roman Empire.</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>This is related to other features that sometimes distinguish parties from other political organizations, including a larger membership, greater stability over time, and a deeper connection to the electorate.</t>
+          <t>It was used by Roman writers to refer to the state and government, even during the period of the Roman Empire.</t>
         </is>
       </c>
     </row>
@@ -2103,22 +2103,22 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>enviroment</t>
+          <t>begining</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>environment</t>
+          <t>Beginning</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>This enviroment encompasses the interaction of all living species, climate, weather and natural resources that affect human survival and economic activity.</t>
+          <t>begining in Italy, and spreading to the rest of Europe by the 16th century, its influence was felt in art, architecture, philosophy, literature, music, science, technology, politics, religion, and other aspects of intellectual inquiry.</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>This environment encompasses the interaction of all living species, climate, weather and natural resources that affect human survival and economic activity.</t>
+          <t>Beginning in Italy, and spreading to the rest of Europe by the 16th century, its influence was felt in art, architecture, philosophy, literature, music, science, technology, politics, religion, and other aspects of intellectual inquiry.</t>
         </is>
       </c>
     </row>
@@ -2130,22 +2130,22 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>immediatly</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>Immediately</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Oxford has educated a wide range of notable alumni, including 31 prime ministers of the United Kingdom and many heads of state and goverment around the world.</t>
+          <t>immediatly after signing the act into law, President George Washington nominated John Jay as the court's new chief justice, and John Rutledge, William Cushing, Robert H.</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Oxford has educated a wide range of notable alumni, including 31 prime ministers of the United Kingdom and many heads of state and government around the world.</t>
+          <t>Immediately after signing the act into law, President George Washington nominated John Jay as the court's new chief justice, and John Rutledge, William Cushing, Robert H.</t>
         </is>
       </c>
     </row>
@@ -2167,12 +2167,12 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>The term "tripartite system" is commonly ascribed to French Enlightenment politcal philosopher Montesquieu, although he did not use such a term but referred to the "distribution" of powers.</t>
+          <t>Socialist politics have been internationalist and nationalist; organised through politcal parties and opposed to party politics; at times overlapping with trade unions and other times independent and critical of them, and present in industrialised and developing nations.</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>The term "tripartite system" is commonly ascribed to French Enlightenment political philosopher Montesquieu, although he did not use such a term but referred to the "distribution" of powers.</t>
+          <t>Socialist politics have been internationalist and nationalist; organised through political parties and opposed to party politics; at times overlapping with trade unions and other times independent and critical of them, and present in industrialised and developing nations.</t>
         </is>
       </c>
     </row>
@@ -2184,22 +2184,22 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>recieve</t>
+          <t>neccessary,</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>receive</t>
+          <t>necessary,</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Based on constitutional provisions empowering the president to appoint and recieve ambassadors and conclude treaties with foreign powers, and on subsequent laws enacted by Congress, the modern presidency has primary responsibility for conducting U.S.</t>
+          <t>If follow-on experiments are neccessary, the routinely scheduled launches of resupply craft allows new hardware to be launched with relative ease.</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Based on constitutional provisions empowering the president to appoint and receive ambassadors and conclude treaties with foreign powers, and on subsequent laws enacted by Congress, the modern presidency has primary responsibility for conducting U.S.</t>
+          <t>If follow-on experiments are necessary, the routinely scheduled launches of resupply craft allows new hardware to be launched with relative ease.</t>
         </is>
       </c>
     </row>
@@ -2211,22 +2211,22 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>begining</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>beginning</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>In an attempt to establish control over the power vacuum in Anatolia, the Allies agreed to launch a Greek peacekeeping force and occupy Smyrna (İzmir), inflaming sectarian tensions and begining the Turkish War of Independence.</t>
+          <t>While there is no legal requirement for the prime minister to be an MP, for practical and politcal reasons the prime minister is expected to win a seat very promptly.</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>In an attempt to establish control over the power vacuum in Anatolia, the Allies agreed to launch a Greek peacekeeping force and occupy Smyrna (İzmir), inflaming sectarian tensions and beginning the Turkish War of Independence.</t>
+          <t>While there is no legal requirement for the prime minister to be an MP, for practical and political reasons the prime minister is expected to win a seat very promptly.</t>
         </is>
       </c>
     </row>
@@ -2248,12 +2248,12 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>The powers, functions and duties of prior presidential offices, in addition to their relation with the prime minister and goverment of Egypt, have over time differed with the various constitutional documents.</t>
+          <t>The moment and place that the phenomenon of human goverment developed is lost in time; however, history does record the formations of early governments.</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>The powers, functions and duties of prior presidential offices, in addition to their relation with the prime minister and government of Egypt, have over time differed with the various constitutional documents.</t>
+          <t>The moment and place that the phenomenon of human government developed is lost in time; however, history does record the formations of early governments.</t>
         </is>
       </c>
     </row>
@@ -2265,22 +2265,22 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>seperate</t>
+          <t>proffesional</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>separate</t>
+          <t>Professional</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Locke distinguishes between seperate powers, but not between discretely separate institutions, and notes that one body or person can share in two or more of the powers.</t>
+          <t>In Hong Kong, Diploma or Advanced Diploma/Certificate (Qualifications Frameworks Level 4), proffesional Diploma/Certificate (Qualifications Frameworks Level 4), higher diploma, and associate degree are below the level of the bachelor's degree.</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Locke distinguishes between separate powers, but not between discretely separate institutions, and notes that one body or person can share in two or more of the powers.</t>
+          <t>In Hong Kong, Diploma or Advanced Diploma/Certificate (Qualifications Frameworks Level 4), Professional Diploma/Certificate (Qualifications Frameworks Level 4), higher diploma, and associate degree are below the level of the bachelor's degree.</t>
         </is>
       </c>
     </row>
@@ -2302,12 +2302,12 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>He launched side ventures, many licensing the Trump name, and filed for six buisness bankruptcies in the 1990s and 2000s.</t>
+          <t>Not restricted to the size of a retail store, Netflix could offer hundreds of thousands of DVDs to customers in a long tail buisness model.</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>He launched side ventures, many licensing the Trump name, and filed for six business bankruptcies in the 1990s and 2000s.</t>
+          <t>Not restricted to the size of a retail store, Netflix could offer hundreds of thousands of DVDs to customers in a long tail business model.</t>
         </is>
       </c>
     </row>
@@ -2319,22 +2319,22 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>goverment.</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>government.</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Although initially committed to non-violent protest, in association with the SACP he co-founded the militant uMkhonto we Sizwe in 1961 that led a sabotage campaign against the apartheid goverment.</t>
+          <t>The prime minister is one of the world's most powerful politcal leaders in modern times.</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Although initially committed to non-violent protest, in association with the SACP he co-founded the militant uMkhonto we Sizwe in 1961 that led a sabotage campaign against the apartheid government.</t>
+          <t>The prime minister is one of the world's most powerful political leaders in modern times.</t>
         </is>
       </c>
     </row>
@@ -2346,22 +2346,22 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>proffesional,</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>professional,</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Historical writing evolved throughout the ages and became increasingly proffesional, particularly during the 19th century, when a rigorous methodology and various academic institutions were established.</t>
+          <t>Autocracies often have a single party that governs the country, and some politcal scientists consider competition between two or more parties to be an essential part of democracy.</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Historical writing evolved throughout the ages and became increasingly professional, particularly during the 19th century, when a rigorous methodology and various academic institutions were established.</t>
+          <t>Autocracies often have a single party that governs the country, and some political scientists consider competition between two or more parties to be an essential part of democracy.</t>
         </is>
       </c>
     </row>
@@ -2373,22 +2373,22 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>immediatly,</t>
+          <t>goverment</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>immediately,</t>
+          <t>government</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>A provisional measure comes into effect immediatly, before Congress votes on it, and remains in force for up to 60 days unless Congress votes to rescind it.</t>
+          <t>The president of the Republic of Korea (Korean: 대한민국 대통령), also known as the president of South Korea (한국 대통령), is the head of state and head of goverment of South Korea.</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>A provisional measure comes into effect immediately, before Congress votes on it, and remains in force for up to 60 days unless Congress votes to rescind it.</t>
+          <t>The president of the Republic of Korea (Korean: 대한민국 대통령), also known as the president of South Korea (한국 대통령), is the head of state and head of government of South Korea.</t>
         </is>
       </c>
     </row>
@@ -2400,22 +2400,22 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>goverment",</t>
+          <t>goverment,</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>government",</t>
+          <t>Government,</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Establishing the provisional "Ankara goverment", he defeated the forces sent by the Allies, thus emerging victorious from the Turkish War of Independence.</t>
+          <t>The research can begin upon the demand of the goverment, political party groups or min 20 MPs.</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Establishing the provisional "Ankara government", he defeated the forces sent by the Allies, thus emerging victorious from the Turkish War of Independence.</t>
+          <t>The research can begin upon the demand of the Government, political party groups or min 20 MPs.</t>
         </is>
       </c>
     </row>
@@ -2427,22 +2427,22 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>begining</t>
+          <t>goverment</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>beginning</t>
+          <t>government</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>The Sultan, begining in 1517, was also a caliph, the leader of all the Sunni Muslims in the world.</t>
+          <t>A goverment is the system or group of people governing an organized community, generally a state.</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>The Sultan, beginning in 1517, was also a caliph, the leader of all the Sunni Muslims in the world.</t>
+          <t>A government is the system or group of people governing an organized community, generally a state.</t>
         </is>
       </c>
     </row>
@@ -2454,22 +2454,22 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>goverment-held</t>
+          <t>goverment</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>government-held</t>
+          <t>government</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Jurisdictions with high levels of transparency are subject to "sunshine laws" or freedom of information legislation that allow citizens broad access to goverment-held information.</t>
+          <t>However, these claims are not accepted by other scholars, who see these forms of goverment as oligarchies.</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Jurisdictions with high levels of transparency are subject to "sunshine laws" or freedom of information legislation that allow citizens broad access to government-held information.</t>
+          <t>However, these claims are not accepted by other scholars, who see these forms of government as oligarchies.</t>
         </is>
       </c>
     </row>
@@ -2481,22 +2481,22 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>politcal</t>
+          <t>goverment.</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Political</t>
+          <t>government.</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>politcal parties in different countries will often adopt similar colours and symbols to identify themselves with a particular ideology.</t>
+          <t>Although initially committed to non-violent protest, in association with the SACP he co-founded the militant uMkhonto we Sizwe in 1961 that led a sabotage campaign against the apartheid goverment.</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Political parties in different countries will often adopt similar colours and symbols to identify themselves with a particular ideology.</t>
+          <t>Although initially committed to non-violent protest, in association with the SACP he co-founded the militant uMkhonto we Sizwe in 1961 that led a sabotage campaign against the apartheid government.</t>
         </is>
       </c>
     </row>
@@ -2518,12 +2518,12 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Liu fell into politcal disgrace during the Cultural Revolution, after which the presidency became vacant.</t>
+          <t>Economic incentives also shape politcal behavior, as certain groups receive more advantages from economic outcomes than others, which allow them to gain political control.</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Liu fell into political disgrace during the Cultural Revolution, after which the presidency became vacant.</t>
+          <t>Economic incentives also shape political behavior, as certain groups receive more advantages from economic outcomes than others, which allow them to gain political control.</t>
         </is>
       </c>
     </row>
@@ -2535,22 +2535,22 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>politcal</t>
+          <t>goverment</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>political</t>
+          <t>government</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Presenting himself as a politcal outsider, Trump won the 2016 presidential election against Democratic Party nominee Hillary Clinton.</t>
+          <t>A nationalist counter goverment led by Mustafa Kemal was established in Ankara when it became clear the Ottoman government was appeasing the Allies.</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Presenting himself as a political outsider, Trump won the 2016 presidential election against Democratic Party nominee Hillary Clinton.</t>
+          <t>A nationalist counter government led by Mustafa Kemal was established in Ankara when it became clear the Ottoman government was appeasing the Allies.</t>
         </is>
       </c>
     </row>
@@ -2562,22 +2562,22 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>neccessary</t>
+          <t>politcal,</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>necessary</t>
+          <t>political,</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>According to Legal Positivists, what law is and what law ought to be have no neccessary connection to one another, so it is theoretically possible to engage in analytic jurisprudence without simultaneously engaging in normative jurisprudence.</t>
+          <t>Panels of experts assess the press freedom score and draft each country summary according to a weighted scoring system that analyzes the politcal, economic, legal and safety situation for journalists based on a 100-point scale.</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>According to Legal Positivists, what law is and what law ought to be have no necessary connection to one another, so it is theoretically possible to engage in analytic jurisprudence without simultaneously engaging in normative jurisprudence.</t>
+          <t>Panels of experts assess the press freedom score and draft each country summary according to a weighted scoring system that analyzes the political, economic, legal and safety situation for journalists based on a 100-point scale.</t>
         </is>
       </c>
     </row>
@@ -2589,22 +2589,22 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>politcal</t>
+          <t>politcal,</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>political</t>
+          <t>political,</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Since 2015, Trump's leadership style and politcal agenda—often referred to as Trumpism—have reshaped the Republican Party's identity.</t>
+          <t>It describes the economic, politcal, and social theories and movements associated with the implementation of such systems.</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Since 2015, Trump's leadership style and political agenda—often referred to as Trumpism—have reshaped the Republican Party's identity.</t>
+          <t>It describes the economic, political, and social theories and movements associated with the implementation of such systems.</t>
         </is>
       </c>
     </row>
@@ -2616,22 +2616,22 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>goverment,</t>
+          <t>goverment</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>government,</t>
+          <t>government</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Such freedom implies no or minimal censorship or prior restraint from goverment, and is often protected by laws or a provision in a constitution.</t>
+          <t>The word goverment derives from the Greek verb κυβερνάω meaning to steer with a gubernaculum (rudder), the metaphorical sense being attested in the literature of classical antiquity, including Plato's Ship of State.</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Such freedom implies no or minimal censorship or prior restraint from government, and is often protected by laws or a provision in a constitution.</t>
+          <t>The word government derives from the Greek verb κυβερνάω meaning to steer with a gubernaculum (rudder), the metaphorical sense being attested in the literature of classical antiquity, including Plato's Ship of State.</t>
         </is>
       </c>
     </row>
@@ -2643,22 +2643,22 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>proffesional,</t>
+          <t>buisness</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>professional,</t>
+          <t>business</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Digital sociology examines the impact of digital technologies on social behavior and institutions, encompassing proffesional, analytical, critical, and public dimensions.</t>
+          <t>He was found guilty in 34 counts of falsifying buisness records in 2024, making him the first U.S.</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Digital sociology examines the impact of digital technologies on social behavior and institutions, encompassing professional, analytical, critical, and public dimensions.</t>
+          <t>He was found guilty in 34 counts of falsifying business records in 2024, making him the first U.S.</t>
         </is>
       </c>
     </row>
@@ -2670,22 +2670,22 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Under the national constitution, the president is also the chief executive of the federal goverment and commander-in-chief of the armed forces.</t>
+          <t>Ancient urban architecture was preoccupied with building religious structures and buildings symbolizing the politcal power of rulers until Greek and Roman architecture shifted focus to civic virtues.</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Under the national constitution, the president is also the chief executive of the federal government and commander-in-chief of the armed forces.</t>
+          <t>Ancient urban architecture was preoccupied with building religious structures and buildings symbolizing the political power of rulers until Greek and Roman architecture shifted focus to civic virtues.</t>
         </is>
       </c>
     </row>
@@ -2697,22 +2697,22 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>seperate</t>
+          <t>goverment</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>separate</t>
+          <t>government</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Gandhi's vision of an independent India based on religious pluralism was challenged in the early 1940s by a Muslim nationalism which demanded a seperate homeland for Muslims within British India.</t>
+          <t>As head of state, the president represents the Turkish goverment to its own people, and represents the nation to the rest of the world.</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Gandhi's vision of an independent India based on religious pluralism was challenged in the early 1940s by a Muslim nationalism which demanded a separate homeland for Muslims within British India.</t>
+          <t>As head of state, the president represents the Turkish government to its own people, and represents the nation to the rest of the world.</t>
         </is>
       </c>
     </row>
@@ -2734,12 +2734,12 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Both, in their roles as goverment leader in the Senate, succeeded prime ministers who had died in office—John A.</t>
+          <t>The presidency is a part of the system of people's congress based on the principle of unified power in which the National People's Congress (NPC) functions as the only branch of goverment and as the supreme state organ of power.</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Both, in their roles as government leader in the Senate, succeeded prime ministers who had died in office—John A.</t>
+          <t>The presidency is a part of the system of people's congress based on the principle of unified power in which the National People's Congress (NPC) functions as the only branch of government and as the supreme state organ of power.</t>
         </is>
       </c>
     </row>
@@ -2751,22 +2751,22 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>politcal</t>
+          <t>goverment,</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>political</t>
+          <t>government,</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>A politcal party is an organization that coordinates candidates to compete in elections and participate in governance.</t>
+          <t>Asquith's Liberal goverment, Churchill was president of the Board of Trade and later Home Secretary, championing prison reform and workers' social security.</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>A political party is an organization that coordinates candidates to compete in elections and participate in governance.</t>
+          <t>Asquith's Liberal government, Churchill was president of the Board of Trade and later Home Secretary, championing prison reform and workers' social security.</t>
         </is>
       </c>
     </row>
@@ -2778,22 +2778,22 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>politcal</t>
+          <t>enviroment.</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>political</t>
+          <t>environment.</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>During the preceding Middle Ages, the European organization of politcal authority was based on a vaguely hierarchical religious order.</t>
+          <t>Globalizing processes affect and are affected by business and work organization, economics, sociocultural resources, and the natural enviroment.</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>During the preceding Middle Ages, the European organization of political authority was based on a vaguely hierarchical religious order.</t>
+          <t>Globalizing processes affect and are affected by business and work organization, economics, sociocultural resources, and the natural environment.</t>
         </is>
       </c>
     </row>
@@ -2805,22 +2805,22 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>neccessary,</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>necessary,</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>If neccessary, the patient may be sent to a medical specialist for further, more detailed examinations.</t>
+          <t>It can also have a social, psychological, spiritual, or politcal role.</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>If necessary, the patient may be sent to a medical specialist for further, more detailed examinations.</t>
+          <t>It can also have a social, psychological, spiritual, or political role.</t>
         </is>
       </c>
     </row>
@@ -2832,22 +2832,22 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>neccessary</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>necessary</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>According to Natural Law Theorists, there is a neccessary connection between what law is and what it ought to be, so it is impossible to engage in analytic jurisprudence without simultaneously engaging in normative jurisprudence.</t>
+          <t>In The Spirit of Law (1748), Montesquieu described the various forms of distribution of politcal power among a legislature, an executive, and a judiciary.</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>According to Natural Law Theorists, there is a necessary connection between what law is and what it ought to be, so it is impossible to engage in analytic jurisprudence without simultaneously engaging in normative jurisprudence.</t>
+          <t>In The Spirit of Law (1748), Montesquieu described the various forms of distribution of political power among a legislature, an executive, and a judiciary.</t>
         </is>
       </c>
     </row>
@@ -2859,22 +2859,22 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>politcal</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>political</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Austria is a parliamentary republic, the system of goverment in which real power is vested in the head of government.</t>
+          <t>Depending on the academic institution, international relations or international affairs is either a subdiscipline of politcal science or a broader multidisciplinary field encompassing global politics, law, economics, or world history.</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Austria is a parliamentary republic, the system of government in which real power is vested in the head of government.</t>
+          <t>Depending on the academic institution, international relations or international affairs is either a subdiscipline of political science or a broader multidisciplinary field encompassing global politics, law, economics, or world history.</t>
         </is>
       </c>
     </row>
@@ -2886,22 +2886,22 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>politcal</t>
+          <t>goverment</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>political</t>
+          <t>government</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Leaders of politcal parties are generally expected to run as a presidential candidate for their party.</t>
+          <t>Advocacy of goverment by a republic is called republicanism, while advocacy of monarchy is called monarchism.</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Leaders of political parties are generally expected to run as a presidential candidate for their party.</t>
+          <t>Advocacy of government by a republic is called republicanism, while advocacy of monarchy is called monarchism.</t>
         </is>
       </c>
     </row>
@@ -2923,12 +2923,12 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Democratic theorists, especially those hoping to achieve more universal suffrage, support presumptive inclusion, where the legal system would protect the voting rights of all subjects unless the goverment can clearly prove that disenfranchisement is necessary.</t>
+          <t>Finally, goverment is also sometimes used in English as a synonym for rule or governance.</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Democratic theorists, especially those hoping to achieve more universal suffrage, support presumptive inclusion, where the legal system would protect the voting rights of all subjects unless the government can clearly prove that disenfranchisement is necessary.</t>
+          <t>Finally, government is also sometimes used in English as a synonym for rule or governance.</t>
         </is>
       </c>
     </row>
@@ -2940,22 +2940,22 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>goverment,</t>
+          <t>independant</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>government,</t>
+          <t>independent</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>If the leader of the opposition is unable or unwilling to form a goverment, the governor general can consult whomever they wish.</t>
+          <t>It says it uses the tools of journalism to help journalists by tracking press freedom issues through independant research, fact-finding missions, and a network of foreign correspondents, including local working journalists in countries worldwide.</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>If the leader of the opposition is unable or unwilling to form a government, the governor general can consult whomever they wish.</t>
+          <t>It says it uses the tools of journalism to help journalists by tracking press freedom issues through independent research, fact-finding missions, and a network of foreign correspondents, including local working journalists in countries worldwide.</t>
         </is>
       </c>
     </row>
@@ -2967,22 +2967,22 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>goverment,</t>
+          <t>enviroment,</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>government,</t>
+          <t>environment,</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Chinese philosophy focuses principally on practical issues about right social conduct, goverment, and self-cultivation.</t>
+          <t>More precisely, we can consider the different aspects or components of an enviroment, and see that their degree of naturalness is not uniform.</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Chinese philosophy focuses principally on practical issues about right social conduct, government, and self-cultivation.</t>
+          <t>More precisely, we can consider the different aspects or components of an environment, and see that their degree of naturalness is not uniform.</t>
         </is>
       </c>
     </row>
@@ -3004,12 +3004,12 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Judges constitute a critical force for judicial interpretation and constitutional review while avoiding politcal bias.</t>
+          <t>By the early 1920s, communism and social democracy had become the two dominant politcal tendencies within the international socialist movement, with socialism itself becoming the most influential secular movement of the 20th century.</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Judges constitute a critical force for judicial interpretation and constitutional review while avoiding political bias.</t>
+          <t>By the early 1920s, communism and social democracy had become the two dominant political tendencies within the international socialist movement, with socialism itself becoming the most influential secular movement of the 20th century.</t>
         </is>
       </c>
     </row>
@@ -3021,22 +3021,22 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>enviroment</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>environment</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>He implemented a strong, well-financed national goverment while remaining impartial in the fierce rivalry that emerged within his cabinet between Thomas Jefferson and Alexander Hamilton.</t>
+          <t>In contrast to the natural enviroment is the built environment.</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>He implemented a strong, well-financed national government while remaining impartial in the fierce rivalry that emerged within his cabinet between Thomas Jefferson and Alexander Hamilton.</t>
+          <t>In contrast to the natural environment is the built environment.</t>
         </is>
       </c>
     </row>
@@ -3053,17 +3053,17 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Government,</t>
+          <t>government,</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>The research can begin upon the demand of the goverment, political party groups or min 20 MPs.</t>
+          <t>Such freedom implies no or minimal censorship or prior restraint from goverment, and is often protected by laws or a provision in a constitution.</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>The research can begin upon the demand of the Government, political party groups or min 20 MPs.</t>
+          <t>Such freedom implies no or minimal censorship or prior restraint from government, and is often protected by laws or a provision in a constitution.</t>
         </is>
       </c>
     </row>
@@ -3075,22 +3075,22 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>politcal</t>
+          <t>goverment</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>political</t>
+          <t>government</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>As a subdiscipline of politcal science, the focus of IR studies lies on the political, diplomatic, and security connections among states, as well as the study of modern international relations within the context of world history.</t>
+          <t>In the 2009 federal election, the CDU obtained the largest share of the vote, and Merkel subsequently formed a coalition goverment with the Free Democratic Party (FDP), an alliance more favourable to the CDU than the grand coalition.</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>As a subdiscipline of political science, the focus of IR studies lies on the political, diplomatic, and security connections among states, as well as the study of modern international relations within the context of world history.</t>
+          <t>In the 2009 federal election, the CDU obtained the largest share of the vote, and Merkel subsequently formed a coalition government with the Free Democratic Party (FDP), an alliance more favourable to the CDU than the grand coalition.</t>
         </is>
       </c>
     </row>
@@ -3102,22 +3102,22 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>succesful</t>
+          <t>goverment</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>successful</t>
+          <t>government</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>William Shakespeare was the son of John Shakespeare, an alderman and a succesful glover (glove-maker) originally from Snitterfield in Warwickshire, and Mary Arden, the daughter of an affluent landowning family that was influential in the Recusant Catholic community.</t>
+          <t>The first head of goverment after the monarchy was the State Chancellor of German-Austria, an office again only held by one person; Karl Renner.</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>William Shakespeare was the son of John Shakespeare, an alderman and a successful glover (glove-maker) originally from Snitterfield in Warwickshire, and Mary Arden, the daughter of an affluent landowning family that was influential in the Recusant Catholic community.</t>
+          <t>The first head of government after the monarchy was the State Chancellor of German-Austria, an office again only held by one person; Karl Renner.</t>
         </is>
       </c>
     </row>
@@ -3129,22 +3129,22 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>seperate</t>
+          <t>succesful</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>separate</t>
+          <t>successful</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Later that year, the Bolsheviks seized power in Russia in the October Revolution; Soviet Russia signed an armistice with the Central Powers in December, followed by a seperate peace in March 1918.</t>
+          <t>In 1984, Disney's shareholders voted Michael Eisner as CEO, who led a reversal of the company's decline through a combination of international theme park expansion and the highly succesful Disney Renaissance period of animation from 1989 to 1999.</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Later that year, the Bolsheviks seized power in Russia in the October Revolution; Soviet Russia signed an armistice with the Central Powers in December, followed by a separate peace in March 1918.</t>
+          <t>In 1984, Disney's shareholders voted Michael Eisner as CEO, who led a reversal of the company's decline through a combination of international theme park expansion and the highly successful Disney Renaissance period of animation from 1989 to 1999.</t>
         </is>
       </c>
     </row>
@@ -3156,22 +3156,22 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>politcal</t>
+          <t>succesful</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Political</t>
+          <t>successful</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>politcal parties are collective entities and activities that organize competitions for political offices.</t>
+          <t>The succesful Turkish War of Independence, led by Mustafa Kemal Atatürk against the occupying Allies, led to the emergence of the Republic of Turkey and the abolition of the sultanate in 1922.</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Political parties are collective entities and activities that organize competitions for political offices.</t>
+          <t>The successful Turkish War of Independence, led by Mustafa Kemal Atatürk against the occupying Allies, led to the emergence of the Republic of Turkey and the abolition of the sultanate in 1922.</t>
         </is>
       </c>
     </row>
@@ -3183,22 +3183,22 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>enviroment</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>environment</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>As head of state, the president represents the Turkish goverment to its own people, and represents the nation to the rest of the world.</t>
+          <t>Though many animals build things to provide a better enviroment for themselves, they are not human, hence beaver dams and the works of mound-building termites are thought of as natural.</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>As head of state, the president represents the Turkish government to its own people, and represents the nation to the rest of the world.</t>
+          <t>Though many animals build things to provide a better environment for themselves, they are not human, hence beaver dams and the works of mound-building termites are thought of as natural.</t>
         </is>
       </c>
     </row>
@@ -3210,22 +3210,22 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>goverment</t>
+          <t>goverment),</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>government),</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Churchill formed a national goverment and oversaw British involvement in the Allied war effort against the Axis powers, resulting in victory in 1945.</t>
+          <t>Turkey is a presidential representative democracy and a constitutional republic within a pluriform multi-party system, in which the president (the head of state and head of goverment), parliament, and judiciary share powers reserved to the national government.</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Churchill formed a national government and oversaw British involvement in the Allied war effort against the Axis powers, resulting in victory in 1945.</t>
+          <t>Turkey is a presidential representative democracy and a constitutional republic within a pluriform multi-party system, in which the president (the head of state and head of government), parliament, and judiciary share powers reserved to the national government.</t>
         </is>
       </c>
     </row>
@@ -3237,22 +3237,22 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>enviroment</t>
+          <t>goverment</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>environment</t>
+          <t>government</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Small uncrewed spacecraft can also provide platforms for experiments, especially those involving zero gravity and exposure to space, but space stations offer a long-term enviroment where studies can be performed potentially for decades, combined with ready access by human researchers.</t>
+          <t>Additionally, although an institutionally distinct organ, the goverment is accountable to parliament.</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Small uncrewed spacecraft can also provide platforms for experiments, especially those involving zero gravity and exposure to space, but space stations offer a long-term environment where studies can be performed potentially for decades, combined with ready access by human researchers.</t>
+          <t>Additionally, although an institutionally distinct organ, the government is accountable to parliament.</t>
         </is>
       </c>
     </row>
@@ -3264,22 +3264,22 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>independant</t>
+          <t>goverment</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>independent</t>
+          <t>government</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>The dissolution of the Russian, German, Austro-Hungarian, and Ottoman empires led to new national boundaries and the creation of new independant states including Poland, Finland, the Baltic states, Czechoslovakia, and Yugoslavia.</t>
+          <t>Another example is the Thirty-fourth goverment of Israel (2015–2019), when Benjamin Netanyahu at one point served as the prime minister and minister of Communications, Foreign Affairs, Regional Cooperation, Economy, Defense and Interior.</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>The dissolution of the Russian, German, Austro-Hungarian, and Ottoman empires led to new national boundaries and the creation of new independent states including Poland, Finland, the Baltic states, Czechoslovakia, and Yugoslavia.</t>
+          <t>Another example is the Thirty-fourth government of Israel (2015–2019), when Benjamin Netanyahu at one point served as the prime minister and minister of Communications, Foreign Affairs, Regional Cooperation, Economy, Defense and Interior.</t>
         </is>
       </c>
     </row>

</xml_diff>